<commit_message>
Fixed the randomizer its needed to be tested
</commit_message>
<xml_diff>
--- a/SF_Working_Plan22_Plan.xlsx
+++ b/SF_Working_Plan22_Plan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
   <si>
     <t>Id</t>
   </si>
@@ -37,100 +37,97 @@
     <t>Office Days Count</t>
   </si>
   <si>
+    <t>GOKHAN BINGOL</t>
+  </si>
+  <si>
+    <t>NW</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>ONUR ERDEN</t>
+  </si>
+  <si>
+    <t>UYGAR ZUBARI</t>
+  </si>
+  <si>
+    <t>Normal Working(Company)</t>
+  </si>
+  <si>
+    <t>OZGUR SELMANOGLU</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Annual Leave</t>
+  </si>
+  <si>
+    <t>MENGUÇ HALIL</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Health Report</t>
+  </si>
+  <si>
     <t>ILKNUR KURBAN</t>
   </si>
   <si>
-    <t>NW</t>
-  </si>
-  <si>
-    <t>SW</t>
+    <t>UL</t>
+  </si>
+  <si>
+    <t>Unpaid Leave</t>
+  </si>
+  <si>
+    <t>VOLKAN BALIKCI</t>
+  </si>
+  <si>
+    <t>Smart Working</t>
+  </si>
+  <si>
+    <t>TAHA ERKAN</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>Public Holiday</t>
+  </si>
+  <si>
+    <t>OZGU TURKMEN</t>
+  </si>
+  <si>
+    <t>ENDER YURDAKOC</t>
+  </si>
+  <si>
+    <t>NILDEN TUTALAR</t>
   </si>
   <si>
     <t>UGUR CAN</t>
   </si>
   <si>
+    <t>ZAFER GULER</t>
+  </si>
+  <si>
+    <t>CAN UGURLU</t>
+  </si>
+  <si>
+    <t>ALI EMRE OK</t>
+  </si>
+  <si>
     <t>GURKAN GUNEY</t>
   </si>
   <si>
-    <t>Normal Working(Company)</t>
-  </si>
-  <si>
-    <t>CAN UGURLU</t>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>Annual Leave</t>
-  </si>
-  <si>
-    <t>ALI EMRE OK</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>Health Report</t>
-  </si>
-  <si>
-    <t>MENGUÇ HALIL</t>
-  </si>
-  <si>
-    <t>UL</t>
-  </si>
-  <si>
-    <t>Unpaid Leave</t>
-  </si>
-  <si>
-    <t>OZGUR SELMANOGLU</t>
-  </si>
-  <si>
-    <t>Smart Working</t>
-  </si>
-  <si>
-    <t>OZGU TURKMEN</t>
-  </si>
-  <si>
-    <t>PH</t>
-  </si>
-  <si>
-    <t>Public Holiday</t>
+    <t>OZGUR SALGINCI</t>
   </si>
   <si>
     <t>GAMZE AKYOL</t>
   </si>
   <si>
-    <t>ZAFER GULER</t>
-  </si>
-  <si>
-    <t>OZGUR SALGINCI</t>
-  </si>
-  <si>
-    <t>NILDEN TUTALAR</t>
-  </si>
-  <si>
     <t>EGE KUTAY YURUSEN</t>
-  </si>
-  <si>
-    <t>UYGAR ZUBARI</t>
-  </si>
-  <si>
-    <t>ONUR ERDEN</t>
-  </si>
-  <si>
-    <t>GOKHAN BINGOL</t>
-  </si>
-  <si>
-    <t>ML</t>
-  </si>
-  <si>
-    <t>TAHA ERKAN</t>
-  </si>
-  <si>
-    <t>VOLKAN BALIKCI</t>
-  </si>
-  <si>
-    <t>ENDER YURDAKOC</t>
   </si>
   <si>
     <t>Normal Working Count:</t>
@@ -149,7 +146,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,11 +195,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9900"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFEECC"/>
       </patternFill>
     </fill>
@@ -226,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -237,7 +229,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,7 +599,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>20019</v>
+        <v>20001</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -625,8 +616,8 @@
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H2" s="3">
         <f>=COUNTIF(C2:G2,"NW")</f>
@@ -634,7 +625,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>20027</v>
+        <v>20015</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -648,11 +639,11 @@
       <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H3" s="3">
         <f>=COUNTIF(C3:G3,"NW")</f>
@@ -660,7 +651,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>20035</v>
+        <v>20016</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -692,7 +683,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>20030</v>
+        <v>20017</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -706,8 +697,8 @@
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>10</v>
@@ -724,13 +715,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>20031</v>
+        <v>20018</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -741,8 +732,8 @@
       <c r="F6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
+      <c r="G6" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H6" s="3">
         <f>=COUNTIF(C6:G6,"NW")</f>
@@ -756,7 +747,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>20018</v>
+        <v>20019</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
@@ -770,8 +761,8 @@
       <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>9</v>
+      <c r="F7" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>9</v>
@@ -788,7 +779,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>20017</v>
+        <v>20020</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
@@ -805,8 +796,8 @@
       <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>10</v>
+      <c r="G8" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H8" s="3">
         <f>=COUNTIF(C8:G8,"NW")</f>
@@ -820,7 +811,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>20022</v>
+        <v>20021</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -837,8 +828,8 @@
       <c r="F9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>10</v>
+      <c r="G9" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H9" s="3">
         <f>=COUNTIF(C9:G9,"NW")</f>
@@ -852,13 +843,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>20062</v>
+        <v>20022</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>10</v>
@@ -878,13 +869,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>20029</v>
+        <v>20023</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>9</v>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>10</v>
@@ -892,11 +883,11 @@
       <c r="E11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>10</v>
+      <c r="F11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H11" s="3">
         <f>=COUNTIF(C11:G11,"NW")</f>
@@ -904,7 +895,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>20047</v>
+        <v>20024</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
@@ -921,8 +912,8 @@
       <c r="F12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>10</v>
+      <c r="G12" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H12" s="3">
         <f>=COUNTIF(C12:G12,"NW")</f>
@@ -930,13 +921,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>20024</v>
+        <v>20027</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>10</v>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>10</v>
@@ -944,8 +935,8 @@
       <c r="E13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>9</v>
+      <c r="F13" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>9</v>
@@ -956,13 +947,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>16000287</v>
+        <v>20029</v>
       </c>
       <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>10</v>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>10</v>
@@ -982,13 +973,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>20016</v>
+        <v>20030</v>
       </c>
       <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
+      <c r="C15" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>10</v>
@@ -996,8 +987,8 @@
       <c r="E15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>9</v>
+      <c r="F15" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>9</v>
@@ -1008,7 +999,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>20015</v>
+        <v>20031</v>
       </c>
       <c r="B16" t="s">
         <v>34</v>
@@ -1022,8 +1013,8 @@
       <c r="E16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>9</v>
+      <c r="F16" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>9</v>
@@ -1034,25 +1025,25 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>20001</v>
+        <v>20035</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>10</v>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H17" s="3">
         <f>=COUNTIF(C17:G17,"NW")</f>
@@ -1060,10 +1051,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>20021</v>
+        <v>20047</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>9</v>
@@ -1074,8 +1065,8 @@
       <c r="E18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>10</v>
+      <c r="F18" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>10</v>
@@ -1086,10 +1077,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>20020</v>
+        <v>20062</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>9</v>
@@ -1100,8 +1091,8 @@
       <c r="E19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>10</v>
+      <c r="F19" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>10</v>
@@ -1112,10 +1103,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>20023</v>
+        <v>16000287</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>9</v>
@@ -1126,8 +1117,8 @@
       <c r="E20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>10</v>
+      <c r="F20" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>10</v>
@@ -1138,21 +1129,21 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="10">
+        <v>39</v>
+      </c>
+      <c r="C21" s="9">
         <f>=COUNTIF(C2:C20,"NW")</f>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <f>=COUNTIF(D2:D20,"NW")</f>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="9">
         <f>=COUNTIF(E2:E20,"NW")</f>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="9">
         <f>=COUNTIF(F2:F20,"NW")</f>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="9">
         <f>=COUNTIF(G2:G20,"NW")</f>
       </c>
       <c r="H21" s="4">

</xml_diff>